<commit_message>
Added beta calc for Hansen panels
</commit_message>
<xml_diff>
--- a/Smith_Collapse_Check.xlsx
+++ b/Smith_Collapse_Check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthill\Documents\MS-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55F0BCC-2FC8-46F8-A618-145C1F65CAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE245F7A-F824-45B0-AAFA-5899DAC26DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="480" windowWidth="21420" windowHeight="12090" xr2:uid="{88A961BB-5585-4FD0-A2DA-BFE39E7EB7C7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{88A961BB-5585-4FD0-A2DA-BFE39E7EB7C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <dimension ref="C2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed(?) smith_v2, made plotters for all pareto fronts
</commit_message>
<xml_diff>
--- a/Smith_Collapse_Check.xlsx
+++ b/Smith_Collapse_Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthill\Documents\MS-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE245F7A-F824-45B0-AAFA-5899DAC26DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6BCC91-58ED-414B-8126-AD2D697A7F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{88A961BB-5585-4FD0-A2DA-BFE39E7EB7C7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>E:</t>
   </si>
@@ -44,54 +44,210 @@
     <t>Mpa</t>
   </si>
   <si>
-    <t>eps:</t>
-  </si>
-  <si>
-    <t>sig:</t>
-  </si>
-  <si>
-    <t>I:</t>
-  </si>
-  <si>
-    <t>c:</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>sig_y:</t>
   </si>
   <si>
-    <t>YldCrv:</t>
-  </si>
-  <si>
-    <t>1/m</t>
-  </si>
-  <si>
-    <t>m4</t>
-  </si>
-  <si>
-    <t>My:</t>
-  </si>
-  <si>
     <t>kN-m</t>
   </si>
   <si>
-    <t>strain:</t>
-  </si>
-  <si>
-    <t>stress:</t>
+    <t>Material Properties:</t>
+  </si>
+  <si>
+    <t>Section Property</t>
+  </si>
+  <si>
+    <t>From midship_section</t>
+  </si>
+  <si>
+    <t>From smith_v2</t>
+  </si>
+  <si>
+    <t>y_NA [m]</t>
+  </si>
+  <si>
+    <t>YldCrv [1/m]</t>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [m]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A [m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ixx [m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>My [kN-m]</t>
+  </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>shift_denom [N]</t>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [m]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [m]</t>
+    </r>
+  </si>
+  <si>
+    <t>Mult:</t>
+  </si>
+  <si>
+    <t>*from smith_v2 w/ EP compression elements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -107,7 +263,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -115,13 +271,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,143 +734,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D959A159-C0DB-4B13-ABD8-EDA207846489}">
-  <dimension ref="C2:J19"/>
+  <dimension ref="C2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.41796875" customWidth="1"/>
+    <col min="4" max="4" width="19.68359375" customWidth="1"/>
+    <col min="5" max="5" width="13.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>71000</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
-        <f>-10</f>
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D4">
+        <v>207</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="6" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3.0833215939911098</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3.0482505777342799</v>
+      </c>
+      <c r="F7" s="15">
+        <f>(E7-D7)/D7</f>
+        <v>-1.1374426957336413E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="16.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="9">
+        <f>5.765-D7</f>
+        <v>2.6816784060088898</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2.7051371997721598</v>
+      </c>
+      <c r="F8" s="15">
+        <f>(E8-D8)/D8</f>
+        <v>8.7478027606537005E-3</v>
+      </c>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="3:8" ht="16.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="9">
+        <f>D7</f>
+        <v>3.0833215939911098</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2.9904391975793998</v>
+      </c>
+      <c r="F9" s="15">
+        <f>(E9-D9)/D9</f>
+        <v>-3.0124135151105437E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="16.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="D10" s="9">
+        <f>MAX(D8:D9)</f>
+        <v>3.0833215939911098</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2.9904391975793998</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" ref="F10:F15" si="0">(E10-D10)/D10</f>
+        <v>-3.0124135151105437E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10">
+        <f>D4/(D10*D3)</f>
+        <v>9.4556888370914615E-4</v>
+      </c>
+      <c r="E11" s="10">
+        <v>9.7493804926928696E-4</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>3.1059784290844598E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.28985289753999899</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.28985289753999999</v>
+      </c>
+      <c r="F12" s="16">
+        <f t="shared" si="0"/>
+        <v>3.4472683579944328E-15</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1.0340780638644</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1.0267222402191101</v>
+      </c>
+      <c r="F13" s="16">
+        <f t="shared" si="0"/>
+        <v>-7.113412325758948E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="14">
+        <f>D11*$D$3*D13*1000</f>
+        <v>69423.234876662696</v>
+      </c>
+      <c r="E14" s="14">
+        <v>71070.3316241024</v>
+      </c>
+      <c r="F14" s="16">
+        <f>(E14-D14)/D14</f>
+        <v>2.3725439334049119E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="18">
+        <f>D12*D3*1000000</f>
+        <v>20579555725.339928</v>
+      </c>
+      <c r="E15" s="18">
+        <v>20579555725.34</v>
+      </c>
+      <c r="F15" s="16">
+        <f t="shared" si="0"/>
+        <v>3.5219053809616586E-15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="19">
+        <v>131731.83889674299</v>
+      </c>
+      <c r="E17" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
-        <f>$D$2*D3</f>
-        <v>-710000</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <f>$D$2*D4</f>
-        <v>710000</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>2.8120328059031201</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>207</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1">
-        <f>D11/(D9*D2)</f>
-        <v>1.036791943403424E-3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13">
-        <v>9.1200000000000005E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14">
-        <f>I13*D2</f>
-        <v>64.75200000000001</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>1.0340780638644</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17">
-        <f>D13*D2*D15*1000</f>
-        <v>76120.790188002313</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I18">
-        <f>-346712.91675593</f>
-        <v>-346712.91675593</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I19">
-        <f>I18/5</f>
-        <v>-69342.583351185996</v>
-      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H22" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>